<commit_message>
validateInputFile spread out over functions
</commit_message>
<xml_diff>
--- a/MijnPythonScripts/Replication_201412.xlsx
+++ b/MijnPythonScripts/Replication_201412.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="60" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="4515" yWindow="120" windowWidth="25605" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -431,7 +431,7 @@
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normaal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Percent 2" xfId="2"/>
   </cellStyles>
@@ -736,74 +736,69 @@
   <dimension ref="A1:CJ11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="22" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="40" max="41" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="55" max="57" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="29" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="55" max="57" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="12" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="70" max="71" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="72" max="73" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="75" max="77" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="81" max="82" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="86" max="87" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="70" max="71" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="72" max="73" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="75" max="77" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="81" max="82" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="86" max="87" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88">
+    <row r="1" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" s="18">
         <v>41974</v>
@@ -1063,7 +1058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:88">
+    <row r="2" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1321,7 +1316,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:88">
+    <row r="3" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>90</v>
       </c>
@@ -1587,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:88">
+    <row r="4" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
@@ -1849,7 +1844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:88">
+    <row r="5" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13" t="s">
@@ -2111,7 +2106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:88">
+    <row r="6" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>90</v>
       </c>
@@ -2377,7 +2372,7 @@
         <v>-5553478.5</v>
       </c>
     </row>
-    <row r="7" spans="1:88">
+    <row r="7" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9" t="s">
@@ -2639,7 +2634,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:88">
+    <row r="8" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13" t="s">
@@ -2901,7 +2896,7 @@
         <v>6.9673586639999989</v>
       </c>
     </row>
-    <row r="9" spans="1:88">
+    <row r="9" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>90</v>
       </c>
@@ -3167,7 +3162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:88">
+    <row r="10" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9" t="s">
@@ -3429,7 +3424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:88">
+    <row r="11" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13" t="s">
@@ -3708,7 +3703,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3726,7 +3721,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>